<commit_message>
Completed MultiCollinearity Handling & Made Gini Normal
</commit_message>
<xml_diff>
--- a/sandbox/feature_iv_trail.xlsx
+++ b/sandbox/feature_iv_trail.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,7 +445,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.02870056546645484</v>
+        <v>0.02679936089249968</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.07867342129999688</v>
+        <v>0.07351096319655509</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -471,11 +471,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>installment</t>
+          <t>annual_inc</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.03307069075838132</v>
+        <v>0.02994436047215786</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -486,11 +486,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>annual_inc</t>
+          <t>dti</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.02563542487977294</v>
+        <v>0.058544180341945</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -501,11 +501,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>dti</t>
+          <t>delinq_2yrs</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.05826107380622716</v>
+        <v>0.006448392208703324</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -516,11 +516,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>delinq_2yrs</t>
+          <t>inq_last_6mths</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.008975621527214699</v>
+        <v>0.06613857212172697</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -531,11 +531,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>inq_last_6mths</t>
+          <t>open_acc</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.05987168026602282</v>
+        <v>0.01833789088814532</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -546,11 +546,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>open_acc</t>
+          <t>pub_rec</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.01596167965604377</v>
+        <v>0.009889452650078862</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -561,11 +561,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>pub_rec</t>
+          <t>revol_util</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01028875169690901</v>
+        <v>0.04586718328110617</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -576,11 +576,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>revol_bal</t>
+          <t>collections_12_mths_ex_med</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.003888723949435664</v>
+        <v>0</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -591,11 +591,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>revol_util</t>
+          <t>acc_now_delinq</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.05057567474927799</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -606,11 +606,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>total_acc</t>
+          <t>total_rev_hi_lim</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.01966623256131316</v>
+        <v>0.04956163577897018</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -621,11 +621,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>collections_12_mths_ex_med</t>
+          <t>acc_open_past_24mths</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>0.09404562766131314</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -636,11 +636,11 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>acc_now_delinq</t>
+          <t>bc_open_to_buy</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>0.0986959598679842</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -651,11 +651,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>tot_cur_bal</t>
+          <t>chargeoff_within_12_mths</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.02361239940071409</v>
+        <v>0</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -666,11 +666,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>total_rev_hi_lim</t>
+          <t>delinq_amnt</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.04585071558922235</v>
+        <v>0</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -681,11 +681,11 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>acc_open_past_24mths</t>
+          <t>mo_sin_old_il_acct</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.09374410030040327</v>
+        <v>0.005737033260385202</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -696,11 +696,11 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>avg_cur_bal</t>
+          <t>mo_sin_rcnt_rev_tl_op</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.03373935714506</v>
+        <v>0.04994750401481346</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -711,11 +711,11 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>bc_open_to_buy</t>
+          <t>mo_sin_rcnt_tl</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1034110147283218</v>
+        <v>0.05906315283323268</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -726,11 +726,11 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>bc_util</t>
+          <t>mort_acc</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.06296514920852986</v>
+        <v>0.01009848359551024</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -741,11 +741,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>chargeoff_within_12_mths</t>
+          <t>mths_since_recent_bc</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>0.03087350977346136</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -756,11 +756,11 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>delinq_amnt</t>
+          <t>mths_since_recent_inq</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0</v>
+        <v>0.04794629682667555</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -771,11 +771,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>mo_sin_old_il_acct</t>
+          <t>num_accts_ever_120_pd</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.00301013773348204</v>
+        <v>0.004224070283564958</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -786,11 +786,11 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>mo_sin_old_rev_tl_op</t>
+          <t>num_actv_bc_tl</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.008203709215265677</v>
+        <v>0.005588981108474164</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -801,11 +801,11 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>mo_sin_rcnt_rev_tl_op</t>
+          <t>num_bc_sats</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.04844163536303294</v>
+        <v>0.0006732742502022557</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -816,11 +816,11 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>mo_sin_rcnt_tl</t>
+          <t>num_bc_tl</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.05500027022196027</v>
+        <v>0.007726510674384336</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -831,11 +831,11 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>mort_acc</t>
+          <t>num_il_tl</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.005850973290228619</v>
+        <v>0.01068682936845326</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -846,11 +846,11 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>mths_since_recent_bc</t>
+          <t>num_sats</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.02682385505881933</v>
+        <v>0.01994252742612374</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -861,11 +861,11 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>mths_since_recent_inq</t>
+          <t>num_tl_120dpd_2m</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.04111979609728165</v>
+        <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -876,11 +876,11 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>num_accts_ever_120_pd</t>
+          <t>num_tl_90g_dpd_24m</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.004248525395214446</v>
+        <v>0.002974867668105873</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -891,11 +891,11 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>num_actv_bc_tl</t>
+          <t>num_tl_op_past_12m</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.004029093195103944</v>
+        <v>0.07615103265561597</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -906,11 +906,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>num_actv_rev_tl</t>
+          <t>pct_tl_nvr_dlq</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.02888335977171912</v>
+        <v>0.009113335428201735</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -921,11 +921,11 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>num_bc_sats</t>
+          <t>pub_rec_bankruptcies</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.0004218288127800436</v>
+        <v>0.005659903310450277</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -936,11 +936,11 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>num_bc_tl</t>
+          <t>tax_liens</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.006352862067195134</v>
+        <v>0</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -951,11 +951,11 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>num_il_tl</t>
+          <t>tot_hi_cred_lim</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.00952716634224076</v>
+        <v>0.04090672067033506</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -966,11 +966,11 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>num_op_rev_tl</t>
+          <t>total_bal_ex_mort</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.01333037282311057</v>
+        <v>0.01330613756016976</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -981,11 +981,11 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>num_rev_accts</t>
+          <t>credit_history_years</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.01800527690685146</v>
+        <v>0.009732800465586871</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -996,11 +996,11 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>num_rev_tl_bal_gt_0</t>
+          <t>fico_score</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.02847620052153776</v>
+        <v>0.166892515183594</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1011,11 +1011,11 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>num_sats</t>
+          <t>proportion_satisfac_accounts</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.01678806730139195</v>
+        <v>0.01232121252120314</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1026,570 +1026,15 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>num_tl_120dpd_2m</t>
+          <t>proportion_satisfac_bc_tl</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>0.008623530086421352</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
           <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>num_tl_30dpd</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>0</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>num_tl_90g_dpd_24m</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>0.004276675944215506</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>num_tl_op_past_12m</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>0.06957747187195878</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>pct_tl_nvr_dlq</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>0.005146185951227811</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>percent_bc_gt_75</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>0.0634257407241266</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>pub_rec_bankruptcies</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>0.004682806505999878</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>tax_liens</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>tot_hi_cred_lim</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>0.03356413330705021</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>total_bal_ex_mort</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>0.01085713238353386</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>total_bc_limit</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>0.06798815014054127</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>total_il_high_credit_limit</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>0.004072560172109733</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>credit_history_years</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>0.004595941524859819</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>fico_score</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>0.1675749104490207</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>last_fico_score</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>4.272018347423384</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>base</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>fico_score_loan_amnt</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>0.0350964976584567</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>installment_term_annual_inc_ratio</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>0.1387878127129355</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>loan_amnt_annual_inc_ratio</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>0.08702490440271195</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>bc_open_to_buy_annual_inc_ratio</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>0.06681836772636043</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>acc_open24m_revol_util</t>
-        </is>
-      </c>
-      <c r="B60" t="n">
-        <v>0.1746902606945003</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>tl_op12m_delinq</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
-        <v>0.01762145050199232</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>tl_op12m_inq6m</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>0.06604158270205078</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>delinq_inq</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>0.01741469328202811</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>rev_limit_annual_inc_ratio</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>0.01128156028195792</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>dti_inq</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>0.08409721259115399</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>dti_fico_ratio</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>0.07389168413414671</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>dti_delinq</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>0</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>dti_revol_util</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>0.08677251863557393</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>revol_util_delinq</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>0.01166076109833241</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>fico_score_revol_util</t>
-        </is>
-      </c>
-      <c r="B70" t="n">
-        <v>0.05940870526518612</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>dti_bc_util</t>
-        </is>
-      </c>
-      <c r="B71" t="n">
-        <v>0.09396099433722765</v>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>loan_amnt_bc_open_to_buy</t>
-        </is>
-      </c>
-      <c r="B72" t="n">
-        <v>0.1291076986230615</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>pct_bc_gt_75_delinq_2yrs</t>
-        </is>
-      </c>
-      <c r="B73" t="n">
-        <v>0.01123012639657948</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>is_verified</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>0.07440016914996586</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>dti_verified_ratio</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>0.0144378825825956</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>dti_verified_multiply</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>0.1143070108407633</v>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>is_fractional</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>0.04775733607857334</v>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>interaction</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>revol_util_fractional</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>0.05889315662822518</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>interaction</t>
         </is>
       </c>
     </row>

</xml_diff>